<commit_message>
agregando pdf y tablas que no se pueden editar
</commit_message>
<xml_diff>
--- a/src/persistencia/pacientes.xlsx
+++ b/src/persistencia/pacientes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2136" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2316" uniqueCount="48">
   <si>
     <t>nick</t>
   </si>
@@ -750,16 +750,16 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
mejorando archivos del programa y corrigiendo credenciales
</commit_message>
<xml_diff>
--- a/src/persistencia/pacientes.xlsx
+++ b/src/persistencia/pacientes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2658" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2814" uniqueCount="71">
   <si>
     <t>nick</t>
   </si>
@@ -184,6 +184,60 @@
   </si>
   <si>
     <t>ASDASD ASDASD</t>
+  </si>
+  <si>
+    <t>21876549</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRENDAN </t>
+  </si>
+  <si>
+    <t>SALINAS  CORTES</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>83946298</t>
+  </si>
+  <si>
+    <t>JANOC</t>
+  </si>
+  <si>
+    <t>MONTES ARIAS</t>
+  </si>
+  <si>
+    <t>97654938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAFAEL </t>
+  </si>
+  <si>
+    <t>PINEDA  MIRANDA</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>34560924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMERIO </t>
+  </si>
+  <si>
+    <t>BORREGO  REYNA</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>23495867</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENIGNA </t>
+  </si>
+  <si>
+    <t>ARMAS  JIMENEZ</t>
   </si>
 </sst>
 </file>
@@ -765,16 +819,16 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>

</xml_diff>